<commit_message>
01-01-2018 : Some Enhancement in forms, Scheduler->Auto Delete Validity Expired Emp, Other Config
</commit_message>
<xml_diff>
--- a/upload_template/BulkSanction_Upload.xlsx
+++ b/upload_template/BulkSanction_Upload.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>InTime</t>
   </si>
@@ -30,27 +30,6 @@
     <t>ShiftCode</t>
   </si>
   <si>
-    <t>GN</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>09:00</t>
-  </si>
-  <si>
-    <t>08:01</t>
-  </si>
-  <si>
-    <t>GI</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>18:01</t>
-  </si>
-  <si>
     <t>EmpUnqID</t>
   </si>
   <si>
@@ -60,31 +39,10 @@
     <t>TPAHours</t>
   </si>
   <si>
-    <t>20:01</t>
-  </si>
-  <si>
-    <t>2017-11-20</t>
-  </si>
-  <si>
-    <t>2017-11-18</t>
-  </si>
-  <si>
-    <t>2017-11-19</t>
-  </si>
-  <si>
-    <t>2017-11-21</t>
-  </si>
-  <si>
-    <t>2017-11-22</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>17:00</t>
+    <t>2017-12-01</t>
+  </si>
+  <si>
+    <t>AA</t>
   </si>
 </sst>
 </file>
@@ -440,7 +398,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,10 +409,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -466,105 +424,44 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20010915</v>
+        <v>20005890</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>20010915</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>20010915</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>4</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>20010915</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>20010915</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2020-10-22 : lots of minore changes
</commit_message>
<xml_diff>
--- a/upload_template/BulkSanction_Upload.xlsx
+++ b/upload_template/BulkSanction_Upload.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance\upload_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25733D1F-5039-4725-B3D3-9ADC9CB2AD55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="19095" windowHeight="8445"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bulk Sanction Format" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>InTime</t>
   </si>
@@ -39,16 +40,37 @@
     <t>TPAHours</t>
   </si>
   <si>
-    <t>2017-12-01</t>
-  </si>
-  <si>
-    <t>AA</t>
+    <t>2020-08-26</t>
+  </si>
+  <si>
+    <t>104019</t>
+  </si>
+  <si>
+    <t>09:00</t>
+  </si>
+  <si>
+    <t>2020-08-25</t>
+  </si>
+  <si>
+    <t>112244</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>Reason</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,6 +206,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -219,6 +258,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -394,20 +450,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -426,42 +483,55 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>20005890</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>